<commit_message>
updated TC and TestActionLibrary for LPH_V1.9.2
</commit_message>
<xml_diff>
--- a/SystemTest/SmokeSanityExecutionResult_LPH_V1.9.1.xlsx
+++ b/SystemTest/SmokeSanityExecutionResult_LPH_V1.9.1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25395" yWindow="0" windowWidth="13905" windowHeight="12300"/>
+    <workbookView xWindow="26460" yWindow="0" windowWidth="13905" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -69,27 +69,27 @@
     <t>Laboratory\TC005GenerateLabReport.py</t>
   </si>
   <si>
+    <t>TC004</t>
+  </si>
+  <si>
+    <t>Radiology\TC001GenerateUSGReport.py</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>Pharmacy\TC003PharmacyOPDbilling.py</t>
+  </si>
+  <si>
+    <t>TC006</t>
+  </si>
+  <si>
+    <t>Pharmacy\Reports\TC010VerifyPharmacyDashboard.py</t>
+  </si>
+  <si>
     <t>Failed</t>
   </si>
   <si>
-    <t>TC004</t>
-  </si>
-  <si>
-    <t>Radiology\TC001GenerateUSGReport.py</t>
-  </si>
-  <si>
-    <t>TC005</t>
-  </si>
-  <si>
-    <t>Pharmacy\TC003PharmacyOPDbilling.py</t>
-  </si>
-  <si>
-    <t>TC006</t>
-  </si>
-  <si>
-    <t>Pharmacy\Reports\TC010VerifyPharmacyDashboard.py</t>
-  </si>
-  <si>
     <t>TC007</t>
   </si>
   <si>
@@ -123,30 +123,48 @@
     <t>TC011</t>
   </si>
   <si>
+    <t>Automation not feasible</t>
+  </si>
+  <si>
+    <t>OnHold</t>
+  </si>
+  <si>
     <t>Reports\TC001BillingDashboardSummary.py</t>
   </si>
   <si>
     <t>TC012</t>
   </si>
   <si>
+    <t>LPH-901</t>
+  </si>
+  <si>
     <t>Billing\OPbilling\TC012CreateCopyOfItemsCreditInvoice.py</t>
   </si>
   <si>
     <t>TC013</t>
   </si>
   <si>
+    <t>Feature Not Available</t>
+  </si>
+  <si>
     <t>Reports\TC003SalesDayBookReport.py</t>
   </si>
   <si>
     <t>TC014</t>
   </si>
   <si>
+    <t>Report Hidden</t>
+  </si>
+  <si>
     <t>Reports\TC005IncomeSegregationReport.py</t>
   </si>
   <si>
     <t>TC016</t>
   </si>
   <si>
+    <t>LPH-866</t>
+  </si>
+  <si>
     <t>Reports\TC006PatientCreditSummaryReport.py</t>
   </si>
   <si>
@@ -163,24 +181,6 @@
   </si>
   <si>
     <t>TC019</t>
-  </si>
-  <si>
-    <t>LPH-901</t>
-  </si>
-  <si>
-    <t>OnHold</t>
-  </si>
-  <si>
-    <t>Feature Not Available</t>
-  </si>
-  <si>
-    <t>Automation not feasible</t>
-  </si>
-  <si>
-    <t>Report Hidden</t>
-  </si>
-  <si>
-    <t>LPH-866</t>
   </si>
   <si>
     <t>LPH-867</t>
@@ -576,7 +576,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,8 +672,8 @@
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -682,7 +682,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="4" t="s">
@@ -691,7 +691,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>8</v>
@@ -703,26 +703,26 @@
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="4" t="s">
@@ -731,16 +731,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>23</v>
@@ -815,119 +815,119 @@
         <v>32</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
@@ -939,59 +939,59 @@
         <v>2</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="3">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="3">
-        <v>4</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="G18" s="7" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>54</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>